<commit_message>
remove duplicated code, add /stats, now /hasentry return number of items found and only first 10 (telegram max size of message is 4096 bytes)
</commit_message>
<xml_diff>
--- a/exceldb-bot/src/test/resources/index.xlsx
+++ b/exceldb-bot/src/test/resources/index.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>cedric walter</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>wwww.galaxiis.com</t>
+  </si>
+  <si>
+    <t>proxeus</t>
+  </si>
+  <si>
+    <t>tech</t>
   </si>
 </sst>
 </file>
@@ -428,11 +434,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:J3"/>
+  <dimension ref="C1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +496,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" xr:uid="{F12B4BEB-AB53-4696-9F71-12869002973A}"/>

</xml_diff>